<commit_message>
pop time series read
</commit_message>
<xml_diff>
--- a/data/stressor_response_demo.xlsx
+++ b/data/stressor_response_demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEA1740-73F4-4F3E-822F-3E8511A92429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36004525-78BF-45BB-A75A-79C50C07A19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="624" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -14230,7 +14230,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>